<commit_message>
Commit current B5 WIP
</commit_message>
<xml_diff>
--- a/LM5060 Design_Calculator_REV_C.xlsx
+++ b/LM5060 Design_Calculator_REV_C.xlsx
@@ -3108,6 +3108,27 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3145,27 +3166,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -9606,8 +9606,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9664,21 +9664,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="83" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="287" t="s">
+      <c r="A1" s="294" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
-      <c r="G1" s="288"/>
-      <c r="H1" s="288"/>
-      <c r="I1" s="288"/>
-      <c r="J1" s="288"/>
-      <c r="K1" s="288"/>
-      <c r="L1" s="288"/>
-      <c r="M1" s="288"/>
+      <c r="B1" s="295"/>
+      <c r="C1" s="295"/>
+      <c r="D1" s="295"/>
+      <c r="E1" s="295"/>
+      <c r="F1" s="295"/>
+      <c r="G1" s="295"/>
+      <c r="H1" s="295"/>
+      <c r="I1" s="295"/>
+      <c r="J1" s="295"/>
+      <c r="K1" s="295"/>
+      <c r="L1" s="295"/>
+      <c r="M1" s="295"/>
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
       <c r="P1" s="42"/>
@@ -9721,8 +9721,8 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="302"/>
-      <c r="M2" s="302"/>
+      <c r="L2" s="289"/>
+      <c r="M2" s="289"/>
       <c r="N2" s="19"/>
       <c r="O2" s="19"/>
       <c r="P2" s="19"/>
@@ -10085,10 +10085,10 @@
       <c r="A11" s="19"/>
       <c r="B11" s="25"/>
       <c r="C11" s="119"/>
-      <c r="D11" s="289" t="s">
+      <c r="D11" s="296" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="290"/>
+      <c r="E11" s="297"/>
       <c r="F11" s="19"/>
       <c r="G11" s="20"/>
       <c r="H11" s="19"/>
@@ -10128,8 +10128,8 @@
       <c r="A12" s="19"/>
       <c r="B12" s="25"/>
       <c r="C12" s="118"/>
-      <c r="D12" s="289"/>
-      <c r="E12" s="290"/>
+      <c r="D12" s="296"/>
+      <c r="E12" s="297"/>
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
       <c r="H12" s="19"/>
@@ -10212,12 +10212,12 @@
         <v>217</v>
       </c>
       <c r="C14" s="263"/>
-      <c r="D14" s="294" t="s">
+      <c r="D14" s="301" t="s">
         <v>216</v>
       </c>
-      <c r="E14" s="294"/>
-      <c r="F14" s="294"/>
-      <c r="G14" s="294"/>
+      <c r="E14" s="301"/>
+      <c r="F14" s="301"/>
+      <c r="G14" s="301"/>
       <c r="H14" s="260"/>
       <c r="I14" s="228"/>
       <c r="J14" s="228"/>
@@ -10255,10 +10255,10 @@
       <c r="A15" s="239"/>
       <c r="B15" s="189"/>
       <c r="C15" s="262"/>
-      <c r="D15" s="295"/>
-      <c r="E15" s="295"/>
-      <c r="F15" s="295"/>
-      <c r="G15" s="295"/>
+      <c r="D15" s="302"/>
+      <c r="E15" s="302"/>
+      <c r="F15" s="302"/>
+      <c r="G15" s="302"/>
       <c r="H15" s="261"/>
       <c r="I15" s="240"/>
       <c r="J15" s="240"/>
@@ -10295,16 +10295,16 @@
     </row>
     <row r="16" spans="1:40" s="238" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="239"/>
-      <c r="B16" s="292"/>
+      <c r="B16" s="299"/>
       <c r="C16" s="244"/>
-      <c r="D16" s="303" t="s">
+      <c r="D16" s="290" t="s">
         <v>218</v>
       </c>
-      <c r="E16" s="303"/>
-      <c r="F16" s="303"/>
-      <c r="G16" s="303"/>
-      <c r="H16" s="303"/>
-      <c r="I16" s="303"/>
+      <c r="E16" s="290"/>
+      <c r="F16" s="290"/>
+      <c r="G16" s="290"/>
+      <c r="H16" s="290"/>
+      <c r="I16" s="290"/>
       <c r="J16" s="247"/>
       <c r="K16" s="242"/>
       <c r="L16" s="240"/>
@@ -10339,16 +10339,16 @@
     </row>
     <row r="17" spans="1:40" s="238" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="239"/>
-      <c r="B17" s="292"/>
+      <c r="B17" s="299"/>
       <c r="C17" s="244"/>
-      <c r="D17" s="303" t="s">
+      <c r="D17" s="290" t="s">
         <v>219</v>
       </c>
-      <c r="E17" s="303"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="303"/>
-      <c r="H17" s="303"/>
-      <c r="I17" s="303"/>
+      <c r="E17" s="290"/>
+      <c r="F17" s="290"/>
+      <c r="G17" s="290"/>
+      <c r="H17" s="290"/>
+      <c r="I17" s="290"/>
       <c r="J17" s="240"/>
       <c r="K17" s="240"/>
       <c r="L17" s="240"/>
@@ -10383,16 +10383,16 @@
     </row>
     <row r="18" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
-      <c r="B18" s="292"/>
+      <c r="B18" s="299"/>
       <c r="C18" s="236"/>
-      <c r="D18" s="303" t="s">
+      <c r="D18" s="290" t="s">
         <v>220</v>
       </c>
-      <c r="E18" s="303"/>
-      <c r="F18" s="303"/>
-      <c r="G18" s="303"/>
-      <c r="H18" s="303"/>
-      <c r="I18" s="303"/>
+      <c r="E18" s="290"/>
+      <c r="F18" s="290"/>
+      <c r="G18" s="290"/>
+      <c r="H18" s="290"/>
+      <c r="I18" s="290"/>
       <c r="J18" s="240"/>
       <c r="K18" s="226"/>
       <c r="L18" s="226"/>
@@ -10426,16 +10426,16 @@
     </row>
     <row r="19" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
-      <c r="B19" s="292"/>
+      <c r="B19" s="299"/>
       <c r="C19" s="236"/>
-      <c r="D19" s="303" t="s">
+      <c r="D19" s="290" t="s">
         <v>221</v>
       </c>
-      <c r="E19" s="303"/>
-      <c r="F19" s="303"/>
-      <c r="G19" s="303"/>
-      <c r="H19" s="303"/>
-      <c r="I19" s="303"/>
+      <c r="E19" s="290"/>
+      <c r="F19" s="290"/>
+      <c r="G19" s="290"/>
+      <c r="H19" s="290"/>
+      <c r="I19" s="290"/>
       <c r="J19" s="240"/>
       <c r="K19" s="226"/>
       <c r="L19" s="226"/>
@@ -10555,11 +10555,11 @@
       <c r="A22" s="19"/>
       <c r="B22" s="229"/>
       <c r="C22" s="226"/>
-      <c r="D22" s="296" t="s">
+      <c r="D22" s="303" t="s">
         <v>223</v>
       </c>
-      <c r="E22" s="297"/>
-      <c r="F22" s="298"/>
+      <c r="E22" s="304"/>
+      <c r="F22" s="305"/>
       <c r="G22" s="273" t="s">
         <v>214</v>
       </c>
@@ -10603,11 +10603,11 @@
       <c r="A23" s="239"/>
       <c r="B23" s="229"/>
       <c r="C23" s="240"/>
-      <c r="D23" s="304" t="s">
+      <c r="D23" s="291" t="s">
         <v>224</v>
       </c>
-      <c r="E23" s="305"/>
-      <c r="F23" s="306"/>
+      <c r="E23" s="292"/>
+      <c r="F23" s="293"/>
       <c r="G23" s="274" t="s">
         <v>214</v>
       </c>
@@ -10649,11 +10649,11 @@
       <c r="A24" s="19"/>
       <c r="B24" s="229"/>
       <c r="C24" s="226"/>
-      <c r="D24" s="299" t="s">
+      <c r="D24" s="306" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="299"/>
-      <c r="F24" s="299"/>
+      <c r="E24" s="306"/>
+      <c r="F24" s="306"/>
       <c r="G24" s="240"/>
       <c r="H24" s="240"/>
       <c r="I24" s="240"/>
@@ -10695,9 +10695,9 @@
       <c r="A25" s="19"/>
       <c r="B25" s="229"/>
       <c r="C25" s="240"/>
-      <c r="D25" s="299"/>
-      <c r="E25" s="299"/>
-      <c r="F25" s="299"/>
+      <c r="D25" s="306"/>
+      <c r="E25" s="306"/>
+      <c r="F25" s="306"/>
       <c r="G25" s="253"/>
       <c r="H25" s="240"/>
       <c r="I25" s="240"/>
@@ -11058,7 +11058,7 @@
     </row>
     <row r="33" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="264"/>
-      <c r="B33" s="293" t="s">
+      <c r="B33" s="300" t="s">
         <v>210</v>
       </c>
       <c r="C33" s="240"/>
@@ -11107,7 +11107,7 @@
     </row>
     <row r="34" spans="1:40" s="238" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="264"/>
-      <c r="B34" s="293"/>
+      <c r="B34" s="300"/>
       <c r="C34" s="240"/>
       <c r="D34" s="240"/>
       <c r="E34" s="78"/>
@@ -11563,7 +11563,7 @@
     </row>
     <row r="44" spans="1:40" ht="13" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
-      <c r="B44" s="291" t="s">
+      <c r="B44" s="298" t="s">
         <v>210</v>
       </c>
       <c r="C44" s="79"/>
@@ -11613,7 +11613,7 @@
     </row>
     <row r="45" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
-      <c r="B45" s="291"/>
+      <c r="B45" s="298"/>
       <c r="C45" s="79"/>
       <c r="D45" s="23"/>
       <c r="E45" s="37" t="s">
@@ -11661,7 +11661,7 @@
     </row>
     <row r="46" spans="1:40" ht="13" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
-      <c r="B46" s="291"/>
+      <c r="B46" s="298"/>
       <c r="C46" s="79"/>
       <c r="D46" s="23"/>
       <c r="E46" s="37" t="s">
@@ -12371,7 +12371,7 @@
         <v>196</v>
       </c>
       <c r="F61" s="209">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G61" s="101" t="s">
         <v>26</v>
@@ -12419,7 +12419,7 @@
       </c>
       <c r="F62" s="210">
         <f>IGATEMAX/(CONE/1000000000)*(COUTMAX/1000000)*1000</f>
-        <v>6200</v>
+        <v>1319.1489361702129</v>
       </c>
       <c r="G62" s="101" t="s">
         <v>192</v>
@@ -12469,7 +12469,7 @@
       </c>
       <c r="F63" s="5">
         <f>IGATEMAX/(CONE/1000000)</f>
-        <v>3.1</v>
+        <v>0.65957446808510645</v>
       </c>
       <c r="G63" s="101" t="s">
         <v>162</v>
@@ -12517,7 +12517,7 @@
       </c>
       <c r="F64" s="28">
         <f>IF(INRUSH="YES",(GVTHHI*(NUMFETS+IF(BBFET="YES",1,0))/1000000000)/IGATEMIN*1000+(CONE/1000000000)*(VINMAX+VGATEMAX)/IGATEMAX*1000,(GVTHHI*(NUMFETS+IF(BBFET="YES",1,0))/1000000000)/IGATEMIN*1000)</f>
-        <v>12.011385199240987</v>
+        <v>53.188804554079688</v>
       </c>
       <c r="G64" s="101" t="s">
         <v>0</v>
@@ -12565,7 +12565,7 @@
       </c>
       <c r="F65" s="28">
         <f>IF(INRUSH="YES",(GVTHHI*(NUMFETS+IF(BBFET="YES",1,0))/1000000000)/IGATETYP*1000+(CONE/1000000000)*(VINNOM+VGATETYP)/IGATETYP*1000,(GVTHHI*(NUMFETS+IF(BBFET="YES",1,0))/1000000000)/IGATETYP*1000)</f>
-        <v>12.708333333333336</v>
+        <v>57.416666666666664</v>
       </c>
       <c r="G65" s="101" t="s">
         <v>0</v>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="F66" s="28">
         <f>IF(INRUSH="YES",(GVTHHI*(NUMFETS+IF(BBFET="YES",1,0))/1000000000)/IGATEMAX*1000+(CONE/1000000000)*(VINMIN+VGATEMIN)/IGATEMIN*1000,(GVTHHI*(NUMFETS+IF(BBFET="YES",1,0))/1000000000)/IGATEMAX*1000)</f>
-        <v>7.8368121442125229</v>
+        <v>35.042694497153704</v>
       </c>
       <c r="G66" s="101" t="s">
         <v>0</v>
@@ -12661,7 +12661,7 @@
       </c>
       <c r="F67" s="215">
         <f>VDSFLTTMEMIN/1000*(ITMRLMAX)/VTMRHMIN*1000000000</f>
-        <v>42.03984819734346</v>
+        <v>186.16081593927893</v>
       </c>
       <c r="G67" s="101" t="s">
         <v>26</v>
@@ -12708,7 +12708,7 @@
         <v>99</v>
       </c>
       <c r="F68" s="211">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="G68" s="101" t="s">
         <v>26</v>
@@ -12756,7 +12756,7 @@
       </c>
       <c r="F69" s="216">
         <f>VTMRHMIN*CTMR/1000000/ITMRLMAX</f>
-        <v>13.428571428571429</v>
+        <v>62.857142857142861</v>
       </c>
       <c r="G69" s="101" t="s">
         <v>0</v>
@@ -12804,7 +12804,7 @@
       </c>
       <c r="F70" s="216">
         <f>VTMRHTYP*CTMR/1000000/ITMRLTYP</f>
-        <v>15.666666666666666</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="G70" s="101" t="s">
         <v>0</v>
@@ -12852,7 +12852,7 @@
       </c>
       <c r="F71" s="216">
         <f>VTMRHMAX*CTMR/1000000/ITMRLMIN</f>
-        <v>23.5</v>
+        <v>110.00000000000001</v>
       </c>
       <c r="G71" s="101" t="s">
         <v>0</v>
@@ -12900,7 +12900,7 @@
       </c>
       <c r="F72" s="216">
         <f>VTMRHMIN*CTMR/1000000/ITMRHMAX</f>
-        <v>7.2307692307692308</v>
+        <v>33.846153846153847</v>
       </c>
       <c r="G72" s="101" t="s">
         <v>0</v>
@@ -12948,7 +12948,7 @@
       </c>
       <c r="F73" s="216">
         <f>VTMRHTYP*CTMR/1000000/ITMRHTYP</f>
-        <v>8.545454545454545</v>
+        <v>40</v>
       </c>
       <c r="G73" s="101" t="s">
         <v>0</v>
@@ -12996,7 +12996,7 @@
       </c>
       <c r="F74" s="216">
         <f>VTMRHMAX*CTMR/1000000/ITMRHMIN</f>
-        <v>11.058823529411764</v>
+        <v>51.764705882352942</v>
       </c>
       <c r="G74" s="101" t="s">
         <v>0</v>
@@ -13977,13 +13977,13 @@
     <row r="94" spans="1:39" ht="26.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="19"/>
       <c r="B94" s="66"/>
-      <c r="C94" s="300" t="s">
+      <c r="C94" s="287" t="s">
         <v>49</v>
       </c>
-      <c r="D94" s="300"/>
-      <c r="E94" s="300"/>
-      <c r="F94" s="300"/>
-      <c r="G94" s="301"/>
+      <c r="D94" s="287"/>
+      <c r="E94" s="287"/>
+      <c r="F94" s="287"/>
+      <c r="G94" s="288"/>
       <c r="H94" s="79"/>
       <c r="I94" s="79"/>
       <c r="J94" s="23"/>
@@ -14020,11 +14020,11 @@
     <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="19"/>
       <c r="B95" s="66"/>
-      <c r="C95" s="300"/>
-      <c r="D95" s="300"/>
-      <c r="E95" s="300"/>
-      <c r="F95" s="300"/>
-      <c r="G95" s="301"/>
+      <c r="C95" s="287"/>
+      <c r="D95" s="287"/>
+      <c r="E95" s="287"/>
+      <c r="F95" s="287"/>
+      <c r="G95" s="288"/>
       <c r="H95" s="79"/>
       <c r="I95" s="79"/>
       <c r="J95" s="23"/>
@@ -14061,11 +14061,11 @@
     <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="19"/>
       <c r="B96" s="66"/>
-      <c r="C96" s="300"/>
-      <c r="D96" s="300"/>
-      <c r="E96" s="300"/>
-      <c r="F96" s="300"/>
-      <c r="G96" s="301"/>
+      <c r="C96" s="287"/>
+      <c r="D96" s="287"/>
+      <c r="E96" s="287"/>
+      <c r="F96" s="287"/>
+      <c r="G96" s="288"/>
       <c r="H96" s="79"/>
       <c r="I96" s="79"/>
       <c r="J96" s="23"/>
@@ -14320,7 +14320,7 @@
       </c>
       <c r="K101" s="89">
         <f>F70</f>
-        <v>15.666666666666666</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="L101" s="163" t="str">
         <f>G70</f>
@@ -14376,7 +14376,7 @@
       </c>
       <c r="K102" s="89">
         <f>F73</f>
-        <v>8.545454545454545</v>
+        <v>40</v>
       </c>
       <c r="L102" s="163" t="str">
         <f>G73</f>
@@ -14640,7 +14640,7 @@
       </c>
       <c r="F107" s="48">
         <f>CTMR</f>
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="G107" s="101" t="s">
         <v>26</v>
@@ -14737,7 +14737,7 @@
       </c>
       <c r="F109" s="49">
         <f>CONE</f>
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G109" s="101" t="s">
         <v>26</v>
@@ -18123,13 +18123,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="C94:G96"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D16:I16"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="D23:F23"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="B44:B46"/>
@@ -18138,6 +18131,13 @@
     <mergeCell ref="D14:G15"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D24:F25"/>
+    <mergeCell ref="C94:G96"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D16:I16"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="D23:F23"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="G83">
@@ -22051,18 +22051,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22082,6 +22082,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F385080-AA43-47B1-B5FC-DE683234294C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F9DA69-AC46-4980-8991-D5FD33AE93E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -22094,12 +22102,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F385080-AA43-47B1-B5FC-DE683234294C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>